<commit_message>
add chart for students score
</commit_message>
<xml_diff>
--- a/02-01/Book1.xlsx
+++ b/02-01/Book1.xlsx
@@ -173,6 +173,260 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <date1904 val="0"/>
+  <lang val="en-US"/>
+  <roundedCorners val="0"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr anchorCtr="false" rot="0" spcFirstLastPara="false"/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="false" baseline="0" i="false" kern="1200" spc="0" strike="noStrike" sz="1400" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr altLang="en-US" b="false" baseline="0" i="false" kern="0" lang="en-US" spc="0"/>
+              <a:t>成绩单</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+      <overlay val="0"/>
+      <spPr/>
+      <txPr>
+        <a:bodyPr anchorCtr="false" rot="0" spcFirstLastPara="false"/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="false" baseline="0" i="false" kern="1200" spc="0" strike="noStrike" sz="14000" u="none"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </txPr>
+    </title>
+    <view3D>
+      <rotX val="0"/>
+      <rotY val="0"/>
+      <rAngAx val="0"/>
+      <perspective val="0"/>
+    </view3D>
+    <floor>
+      <thickness val="0"/>
+    </floor>
+    <sideWall>
+      <thickness val="0"/>
+    </sideWall>
+    <backWall>
+      <thickness val="0"/>
+    </backWall>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>成绩单!$A$2</f>
+            </strRef>
+          </tx>
+          <dLbls>
+            <showLegendKey val="0"/>
+            <showVal val="0"/>
+            <showCatName val="0"/>
+            <showSerName val="0"/>
+            <showPercent val="0"/>
+            <showBubbleSize val="0"/>
+            <showLeaderLines val="0"/>
+          </dLbls>
+          <invertIfNegative val="0"/>
+          <cat>
+            <strRef>
+              <f>成绩单!$C$4:$C$9</f>
+            </strRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>成绩单!$J$4:$J$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <dLbls>
+          <showLegendKey val="0"/>
+          <showVal val="0"/>
+          <showCatName val="0"/>
+          <showSerName val="0"/>
+          <showPercent val="0"/>
+          <showBubbleSize val="0"/>
+          <showLeaderLines val="0"/>
+        </dLbls>
+        <axId val="754001152"/>
+        <axId val="753999904"/>
+      </barChart>
+      <catAx>
+        <axId val="754001152"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="b"/>
+        <numFmt formatCode="General" sourceLinked="true"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr anchor="ctr" anchorCtr="true" rot="-60000000" spcFirstLastPara="true" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="false" baseline="0" i="false" kern="1200" spc="0" strike="noStrike" sz="900" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="15000"/>
+                    <a:lumOff val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </txPr>
+        <crossAx val="753999904"/>
+        <crosses val="autoZero"/>
+        <auto val="1"/>
+        <lblAlgn val="ctr"/>
+        <lblOffset val="100"/>
+        <noMultiLvlLbl val="0"/>
+      </catAx>
+      <valAx>
+        <axId val="753999904"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <delete val="0"/>
+        <axPos val="l"/>
+        <numFmt formatCode="General" sourceLinked="true"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <tickLblPos val="nextTo"/>
+        <spPr>
+          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </spPr>
+        <txPr>
+          <a:bodyPr anchor="ctr" anchorCtr="true" rot="-60000000" spcFirstLastPara="true" vert="horz" vertOverflow="ellipsis" wrap="square"/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="false" baseline="0" i="false" kern="1200" spc="0" strike="noStrike" sz="900" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="15000"/>
+                    <a:lumOff val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </txPr>
+        <crossAx val="754001152"/>
+        <crosses val="autoZero"/>
+        <crossBetween val="between"/>
+      </valAx>
+    </plotArea>
+    <plotVisOnly val="0"/>
+    <dispBlanksAs val="gap"/>
+    <showDLblsOverMax val="0"/>
+  </chart>
+  <spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </a:ln>
+  </spPr>
+  <printSettings>
+    <pageMargins b="0.75" footer="0.3" header="0.3" l="0.7" r="0.7" t="0.7"/>
+  </printSettings>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" descr=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="false" fPrintsWithSheet="true"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -730,6 +984,7 @@
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H2:J2"/>
   </mergeCells>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>